<commit_message>
main: ``` Refactored plotting functions and updated data files for car price analysis
- Implemented two new plotting functions for better data visualization: plot_price_vs_year and plot_price_vs_mileage
- Added new Excel and PNG data files for Audi TT S Line, Audi TTS, Mini S 5 Door, and Mini S Convertible models
- Renamed a PNG file for consistency in naming convention
- Removed old data files for Audi TTS and Cooper S 5 Door models
- Updated requirements.txt with new library versions
```
</commit_message>
<xml_diff>
--- a/audi_tts.xlsx
+++ b/audi_tts.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcfasel/git/car_graph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B3782D-E693-AE4D-B4D7-CE3EA6B308AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E8299F-A189-1646-AD95-8B31B9154A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{E430248E-0659-4C43-B5C8-094979A09CED}"/>
+    <workbookView xWindow="16820" yWindow="8900" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{E430248E-0659-4C43-B5C8-094979A09CED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Audi TTS" sheetId="1" r:id="rId1"/>
+    <sheet name="Audi TT Sport" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -479,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA962B88-8C59-D541-A09D-ED0073DD5D7C}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,64 +724,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2015</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>47980</v>
-      </c>
-      <c r="E9" s="2">
-        <v>46000</v>
-      </c>
-      <c r="F9" s="2">
-        <v>62500</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2016</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10">
-        <v>38670</v>
-      </c>
-      <c r="E10" s="2">
-        <v>37500</v>
-      </c>
-      <c r="F10" s="2">
-        <v>93200</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -965,4 +908,109 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B89363D-4928-BA4F-A3EC-F07357D50DE1}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2015</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>47980</v>
+      </c>
+      <c r="E2" s="2">
+        <v>46000</v>
+      </c>
+      <c r="F2" s="2">
+        <v>62500</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2016</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>38670</v>
+      </c>
+      <c r="E3" s="2">
+        <v>37500</v>
+      </c>
+      <c r="F3" s="2">
+        <v>93200</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>